<commit_message>
rq kernel new try
</commit_message>
<xml_diff>
--- a/src/inputs/time_anly_logs.xlsx
+++ b/src/inputs/time_anly_logs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Documents\bezerkeley\research\isol-sys-database\src\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hpham09\Documents\bezerkeley\research\isol-sys-database\src\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A9D1EB-C7E8-4409-BA67-FE2D74FC9296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52738FAB-E725-4F24-8861-75047EE8675C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,12 +29,15 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
   <si>
     <t>Run name</t>
   </si>
@@ -184,6 +187,12 @@
   </si>
   <si>
     <t>[7, 10, 10, 10]</t>
+  </si>
+  <si>
+    <t>_ta_rq</t>
+  </si>
+  <si>
+    <t>Same as above, but with RQ kernel</t>
   </si>
 </sst>
 </file>
@@ -508,7 +517,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,7 +739,24 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C13" s="2"/>
+      <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="1">
+        <v>45909</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C14" s="2"/>

</xml_diff>

<commit_message>
tweaked cbf enhanced designs via constr
</commit_message>
<xml_diff>
--- a/src/inputs/time_anly_logs.xlsx
+++ b/src/inputs/time_anly_logs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/huy_g_pham_ubc_ca/Documents/Documents/bezerkeley/research/isol-sys-database/src/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{52738FAB-E725-4F24-8861-75047EE8675C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3504993C-0BE0-4C1C-8E5D-ECFC4A0C5F8D}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{52738FAB-E725-4F24-8861-75047EE8675C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA61A0E3-9321-4819-9D03-68AEB3683D64}"/>
   <bookViews>
-    <workbookView xWindow="6435" yWindow="3255" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="59">
   <si>
     <t>Run name</t>
   </si>
@@ -198,13 +198,22 @@
     <t>_complete_spectracomments</t>
   </si>
   <si>
-    <t>[-6, -6, -6, -6]; [-6, -6, -6.2, -7]</t>
-  </si>
-  <si>
     <t>Inv loss run. MF-LRB enhanced repl target increased to 6%</t>
   </si>
   <si>
     <t>[10, 10, 7, 10]; [10, 10, 10, 10]</t>
+  </si>
+  <si>
+    <t>_complete_spectracomments_fixededp</t>
+  </si>
+  <si>
+    <t>Initial P-58 runs use "generate" mode: 1 EDP per run because it mirrors validation.</t>
+  </si>
+  <si>
+    <t>[-6, -6, -6, -6]; [-6, -6.2, -6, -7]</t>
+  </si>
+  <si>
+    <t>[-6, -6, -6, -6]; [-6, -6.5, -6, -7]</t>
   </si>
 </sst>
 </file>
@@ -526,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -802,13 +811,30 @@
         <v>45959</v>
       </c>
       <c r="C23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" t="s">
         <v>54</v>
       </c>
-      <c r="D23" t="s">
-        <v>53</v>
-      </c>
-      <c r="E23" t="s">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>55</v>
+      </c>
+      <c r="B24" s="1">
+        <v>45961</v>
+      </c>
+      <c r="C24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cbf-lrb updated with smaller ry
</commit_message>
<xml_diff>
--- a/src/inputs/time_anly_logs.xlsx
+++ b/src/inputs/time_anly_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/huy_g_pham_ubc_ca/Documents/Documents/bezerkeley/research/isol-sys-database/src/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{52738FAB-E725-4F24-8861-75047EE8675C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1F825FD-038D-4ABE-B204-3BCFB0EC53F4}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{52738FAB-E725-4F24-8861-75047EE8675C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65FB42A0-FA95-42C3-B8D6-5D49241AD121}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -213,10 +213,10 @@
     <t>[-6, -6, -6, -6]; [-6, -6.2, -6, -7]</t>
   </si>
   <si>
-    <t>[-6, -6, -6, -6]; [-6, -6.5, -6, -6]</t>
-  </si>
-  <si>
     <t>[10, 10, 7, 10]; [10, 10, 7, 10]</t>
+  </si>
+  <si>
+    <t>[-6, -6, -6, -6]; [-6, -6.5, -6, -5.8]</t>
   </si>
 </sst>
 </file>
@@ -541,7 +541,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,10 +834,10 @@
         <v>56</v>
       </c>
       <c r="D24" t="s">
+        <v>59</v>
+      </c>
+      <c r="E24" t="s">
         <v>58</v>
-      </c>
-      <c r="E24" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>